<commit_message>
Major performance improvements when dealing with conditional formats. Minor performance improvements across the board.
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/AutoFilter/CustomAutoFilter.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/AutoFilter/CustomAutoFilter.xlsx
@@ -58,7 +58,21 @@
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="1">
+  <x:fonts count="3">
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
     <x:font>
       <x:vertAlign val="baseline"/>
       <x:sz val="11"/>

</xml_diff>

<commit_message>
Fixed issue when copying rows/columns where the format is not always preserved.
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/AutoFilter/CustomAutoFilter.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/AutoFilter/CustomAutoFilter.xlsx
@@ -415,7 +415,7 @@
   </x:sheetPr>
   <x:dimension ref="A1:A7"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="0" workbookViewId="0"/>
+    <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
@@ -481,7 +481,7 @@
   </x:sheetPr>
   <x:dimension ref="A1:A7"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="0" workbookViewId="0"/>
+    <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
@@ -547,7 +547,7 @@
   </x:sheetPr>
   <x:dimension ref="A1:A7"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="0" workbookViewId="0"/>
+    <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
@@ -612,7 +612,7 @@
   </x:sheetPr>
   <x:dimension ref="A1:C7"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="0" workbookViewId="0"/>
+    <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>

</xml_diff>